<commit_message>
Remap stepper disable and spindle enable
</commit_message>
<xml_diff>
--- a/Microcontroller Pin Mapping.xlsx
+++ b/Microcontroller Pin Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quinton\Documents\Personal Projects\Eric CNC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quinton\Documents\Personal Projects\Eric CNC\grblMod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42266C58-BC3B-4CC3-A576-E631A0A913FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D49E22E-D3EC-49A7-8B7E-F82FB7D7F2B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-39555" yWindow="-6540" windowWidth="21600" windowHeight="11265" xr2:uid="{6C2DFAD7-625C-46F2-ADA5-420F2B9264BA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6C2DFAD7-625C-46F2-ADA5-420F2B9264BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Pin Map" sheetId="1" r:id="rId1"/>
@@ -793,12 +793,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1123,8 +1129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BA0AB15-72D4-46DA-AF1B-7586F710B0CD}">
   <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="E89" sqref="E89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1137,24 +1143,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="E1" s="3"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -1298,6 +1304,9 @@
       <c r="D12" s="1" t="s">
         <v>152</v>
       </c>
+      <c r="E12" s="4" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
@@ -1393,6 +1402,7 @@
       <c r="D19" s="1" t="s">
         <v>183</v>
       </c>
+      <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
@@ -1404,9 +1414,7 @@
       <c r="C20" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>105</v>
-      </c>
+      <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
@@ -1418,9 +1426,6 @@
       <c r="C21" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>104</v>
-      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
@@ -1659,6 +1664,9 @@
       </c>
       <c r="D40" s="1" t="s">
         <v>142</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -2478,7 +2486,7 @@
         <f>IF(ISBLANK('Pin Map'!$E28),"",'Pin Map'!$E28)</f>
         <v/>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="6" t="s">
         <v>234</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -2490,7 +2498,7 @@
       </c>
       <c r="H3" s="1" t="str">
         <f>IF(ISBLANK('Pin Map'!$E12),"",'Pin Map'!$E12)</f>
-        <v/>
+        <v>SPINDLE ENABLE</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>213</v>
@@ -2512,7 +2520,7 @@
       </c>
       <c r="P3" s="1" t="str">
         <f>IF(ISBLANK('Pin Map'!$E12),"",'Pin Map'!$E12)</f>
-        <v/>
+        <v>SPINDLE ENABLE</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
@@ -2527,7 +2535,7 @@
         <f>IF(ISBLANK('Pin Map'!$E29),"",'Pin Map'!$E29)</f>
         <v/>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="6"/>
       <c r="F4" s="1" t="s">
         <v>153</v>
       </c>
@@ -2573,7 +2581,7 @@
         <f>IF(ISBLANK('Pin Map'!$E30),"",'Pin Map'!$E30)</f>
         <v/>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="6"/>
       <c r="F5" s="1" t="s">
         <v>200</v>
       </c>
@@ -2617,7 +2625,7 @@
         <f>IF(ISBLANK('Pin Map'!$E31),"",'Pin Map'!$E31)</f>
         <v/>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="1" t="s">
         <v>201</v>
       </c>
@@ -2659,9 +2667,9 @@
       </c>
       <c r="C7" s="1" t="str">
         <f>IF(ISBLANK('Pin Map'!$E40),"",'Pin Map'!$E40)</f>
-        <v/>
-      </c>
-      <c r="E7" s="4"/>
+        <v>STEPPERS DISABLE</v>
+      </c>
+      <c r="E7" s="6"/>
       <c r="F7" s="1" t="s">
         <v>202</v>
       </c>
@@ -2707,7 +2715,7 @@
         <f>IF(ISBLANK('Pin Map'!$E41),"",'Pin Map'!$E41)</f>
         <v/>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="6"/>
       <c r="F8" s="1" t="s">
         <v>203</v>
       </c>
@@ -2753,7 +2761,7 @@
         <f>IF(ISBLANK('Pin Map'!$E42),"",'Pin Map'!$E42)</f>
         <v/>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="6"/>
       <c r="F9" s="1" t="s">
         <v>119</v>
       </c>
@@ -2797,7 +2805,7 @@
         <f>IF(ISBLANK('Pin Map'!$E43),"",'Pin Map'!$E43)</f>
         <v/>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="6"/>
       <c r="F10" s="1" t="s">
         <v>120</v>
       </c>
@@ -2832,7 +2840,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="6" t="s">
         <v>235</v>
       </c>
       <c r="F11" s="1" t="s">
@@ -2869,7 +2877,7 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="E12" s="4"/>
+      <c r="E12" s="6"/>
       <c r="F12" s="1" t="s">
         <v>205</v>
       </c>
@@ -2904,7 +2912,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="E13" s="4"/>
+      <c r="E13" s="6"/>
       <c r="F13" s="1" t="s">
         <v>206</v>
       </c>
@@ -2937,7 +2945,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="E14" s="4"/>
+      <c r="E14" s="6"/>
       <c r="F14" s="1" t="s">
         <v>182</v>
       </c>
@@ -2970,7 +2978,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="E15" s="4"/>
+      <c r="E15" s="6"/>
       <c r="F15" s="1" t="s">
         <v>176</v>
       </c>
@@ -2994,7 +3002,7 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="E16" s="4"/>
+      <c r="E16" s="6"/>
       <c r="F16" s="1" t="s">
         <v>177</v>
       </c>
@@ -3014,11 +3022,11 @@
       </c>
       <c r="L16" s="1" t="str">
         <f>IF(ISBLANK('Pin Map'!$E40),"",'Pin Map'!$E40)</f>
-        <v/>
+        <v>STEPPERS DISABLE</v>
       </c>
     </row>
     <row r="17" spans="5:12" x14ac:dyDescent="0.35">
-      <c r="E17" s="4"/>
+      <c r="E17" s="6"/>
       <c r="F17" s="1" t="s">
         <v>178</v>
       </c>
@@ -3042,7 +3050,7 @@
       </c>
     </row>
     <row r="18" spans="5:12" x14ac:dyDescent="0.35">
-      <c r="E18" s="4"/>
+      <c r="E18" s="6"/>
       <c r="F18" s="1" t="s">
         <v>179</v>
       </c>
@@ -3065,7 +3073,7 @@
       </c>
     </row>
     <row r="19" spans="5:12" x14ac:dyDescent="0.35">
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="6" t="s">
         <v>236</v>
       </c>
       <c r="F19" s="1" t="s">
@@ -3091,7 +3099,7 @@
       </c>
     </row>
     <row r="20" spans="5:12" x14ac:dyDescent="0.35">
-      <c r="E20" s="4"/>
+      <c r="E20" s="6"/>
       <c r="F20" s="1" t="s">
         <v>207</v>
       </c>
@@ -3115,7 +3123,7 @@
       </c>
     </row>
     <row r="21" spans="5:12" x14ac:dyDescent="0.35">
-      <c r="E21" s="4"/>
+      <c r="E21" s="6"/>
       <c r="F21" s="1" t="s">
         <v>209</v>
       </c>
@@ -3139,7 +3147,7 @@
       </c>
     </row>
     <row r="22" spans="5:12" x14ac:dyDescent="0.35">
-      <c r="E22" s="4"/>
+      <c r="E22" s="6"/>
       <c r="F22" s="1" t="s">
         <v>210</v>
       </c>
@@ -3163,7 +3171,7 @@
       </c>
     </row>
     <row r="23" spans="5:12" x14ac:dyDescent="0.35">
-      <c r="E23" s="4"/>
+      <c r="E23" s="6"/>
       <c r="F23" s="1" t="s">
         <v>132</v>
       </c>
@@ -3187,7 +3195,7 @@
       </c>
     </row>
     <row r="24" spans="5:12" x14ac:dyDescent="0.35">
-      <c r="E24" s="4"/>
+      <c r="E24" s="6"/>
       <c r="F24" s="1" t="s">
         <v>211</v>
       </c>
@@ -3211,7 +3219,7 @@
       </c>
     </row>
     <row r="25" spans="5:12" x14ac:dyDescent="0.35">
-      <c r="E25" s="4"/>
+      <c r="E25" s="6"/>
       <c r="F25" s="1" t="s">
         <v>212</v>
       </c>
@@ -3235,7 +3243,7 @@
       </c>
     </row>
     <row r="26" spans="5:12" x14ac:dyDescent="0.35">
-      <c r="E26" s="4"/>
+      <c r="E26" s="6"/>
       <c r="F26" s="1" t="s">
         <v>135</v>
       </c>

</xml_diff>